<commit_message>
Added comprehensive error messaging. Started adding tests.
</commit_message>
<xml_diff>
--- a/src/test/resources/example.xlsx
+++ b/src/test/resources/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/earl/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudorgroza/Work/Phen-X_AI/validator/Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C91C3494-549B-2646-92B1-8DE89EC20A03}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AB5074-6A9B-BC4A-8027-BEF95D612582}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31260" yWindow="4780" windowWidth="20480" windowHeight="12340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="studies" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="101">
   <si>
     <t>A unique free-text label for each genome-wide association study in the publication</t>
   </si>
@@ -286,12 +286,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>rs6487504</t>
-  </si>
-  <si>
-    <t>rs324498</t>
-  </si>
-  <si>
     <t>rs12228810</t>
   </si>
   <si>
@@ -329,13 +323,16 @@
   </si>
   <si>
     <t>Replication</t>
+  </si>
+  <si>
+    <t>Germany</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,6 +374,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -404,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -416,6 +420,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,7 +763,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:Z6"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -861,7 +866,7 @@
     </row>
     <row r="5" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
         <v>80</v>
@@ -878,7 +883,7 @@
       </c>
       <c r="G5"/>
       <c r="H5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I5" t="s">
         <v>83</v>
@@ -905,7 +910,7 @@
     </row>
     <row r="6" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
         <v>80</v>
@@ -920,7 +925,7 @@
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I6" t="s">
         <v>83</v>
@@ -952,11 +957,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:Z11"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1065,26 +1070,24 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>85</v>
       </c>
       <c r="D5" s="5">
-        <v>4.0000000000000001E-8</v>
-      </c>
+        <v>2.9999999999999999E-7</v>
+      </c>
+      <c r="E5" s="4"/>
       <c r="G5" s="4" t="s">
         <v>86</v>
       </c>
       <c r="H5" s="4"/>
+      <c r="I5" s="4">
+        <v>0.69</v>
+      </c>
       <c r="J5" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="M5" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="N5" s="4">
-        <v>1.9</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -1095,20 +1098,18 @@
         <v>87</v>
       </c>
       <c r="D6" s="5">
-        <v>1.9999999999999999E-7</v>
-      </c>
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="E6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H6" s="4"/>
+      <c r="I6" s="4">
+        <v>0.88</v>
+      </c>
       <c r="J6" s="4">
-        <v>1.81</v>
-      </c>
-      <c r="M6" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="N6" s="4">
-        <v>2.2999999999999998</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -1116,34 +1117,33 @@
         <v>93</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D7" s="5">
-        <v>9.9999999999999995E-7</v>
-      </c>
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="E7" s="4"/>
       <c r="G7" s="4" t="s">
         <v>86</v>
       </c>
       <c r="H7" s="4"/>
+      <c r="I7" s="4">
+        <v>0.08</v>
+      </c>
       <c r="J7" s="4">
-        <v>1.62</v>
-      </c>
-      <c r="M7" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="N7" s="4">
-        <v>2</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>95</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D8" s="5">
-        <v>2.9999999999999999E-7</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="E8" s="4"/>
       <c r="G8" s="4" t="s">
@@ -1151,76 +1151,9 @@
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4">
-        <v>0.69</v>
+        <v>0.74</v>
       </c>
       <c r="J8" s="4">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="5">
-        <v>9.0000000000000002E-6</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="G9" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4">
-        <v>0.88</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="5">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="G10" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4">
-        <v>0.08</v>
-      </c>
-      <c r="J10" s="4">
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="5">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="G11" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4">
-        <v>0.74</v>
-      </c>
-      <c r="J11" s="4">
         <v>0.92</v>
       </c>
     </row>
@@ -1235,7 +1168,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1314,10 +1247,10 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" s="4">
         <v>657</v>
@@ -1329,10 +1262,13 @@
         <v>431</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
+      <c r="J5" t="s">
+        <v>100</v>
+      </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="O5" s="4"/>
@@ -1354,10 +1290,10 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6" s="4">
         <v>537</v>
@@ -1369,12 +1305,15 @@
         <v>394</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" t="s">
         <v>100</v>
       </c>
-      <c r="I6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="O6" s="4"/>
@@ -1396,10 +1335,10 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C7" s="4">
         <v>263</v>
@@ -1411,10 +1350,13 @@
         <v>192</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
+      <c r="J7" t="s">
+        <v>100</v>
+      </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="O7" s="4"/>
@@ -1436,10 +1378,10 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C8" s="4">
         <v>322</v>
@@ -1451,12 +1393,15 @@
         <v>192</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" t="s">
         <v>100</v>
       </c>
-      <c r="I8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="O8" s="4"/>
@@ -1478,10 +1423,10 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="C9" s="4">
         <v>920</v>
@@ -1493,10 +1438,13 @@
         <v>623</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
+      <c r="J9" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -1519,10 +1467,10 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="C10" s="4">
         <v>859</v>
@@ -1534,12 +1482,15 @@
         <v>633</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="I10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -1562,10 +1513,10 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C11" s="4">
         <v>2417</v>
@@ -1577,9 +1528,12 @@
         <v>471</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I11" s="4"/>
+      <c r="J11" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>

</xml_diff>